<commit_message>
interim completed the 12f data file read functionality
</commit_message>
<xml_diff>
--- a/data/FOV-optimisation-parameters.xlsx
+++ b/data/FOV-optimisation-parameters.xlsx
@@ -16,23 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Sensor</t>
   </si>
   <si>
-    <t>VisA</t>
-  </si>
-  <si>
-    <t>VisB</t>
-  </si>
-  <si>
-    <t>MwirA</t>
-  </si>
-  <si>
-    <t>MwirB</t>
-  </si>
-  <si>
     <t>Sensor Type</t>
   </si>
   <si>
@@ -72,15 +60,9 @@
     <t>Aberration size factor</t>
   </si>
   <si>
-    <t>Optical transittance</t>
-  </si>
-  <si>
     <t>Frame rate</t>
   </si>
   <si>
-    <t>RMS jitter</t>
-  </si>
-  <si>
     <t>F-number limit</t>
   </si>
   <si>
@@ -121,6 +103,27 @@
   </si>
   <si>
     <t>Central 0.25</t>
+  </si>
+  <si>
+    <t>RMS jitter rad</t>
+  </si>
+  <si>
+    <t>Linear smear rad/s</t>
+  </si>
+  <si>
+    <t>Optical transmittance</t>
+  </si>
+  <si>
+    <t>Vis Sensor A</t>
+  </si>
+  <si>
+    <t>Vis Sensor B</t>
+  </si>
+  <si>
+    <t>MWIR Sensor B</t>
+  </si>
+  <si>
+    <t>MWIR Sensor A</t>
   </si>
 </sst>
 </file>
@@ -464,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -481,55 +484,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>4.7999999999999996E-7</v>
@@ -546,7 +549,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>5.9999999999999997E-7</v>
@@ -563,7 +566,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>1280</v>
@@ -580,7 +583,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>720</v>
@@ -597,7 +600,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
         <v>5.4999999999999999E-6</v>
@@ -614,7 +617,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>0.98</v>
@@ -631,7 +634,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>0.25</v>
@@ -648,7 +651,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>13500</v>
@@ -665,7 +668,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>0.2</v>
@@ -682,7 +685,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>0.25</v>
@@ -699,41 +702,41 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1">
         <v>0.23</v>
@@ -750,7 +753,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>0.5</v>
@@ -767,7 +770,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1">
         <v>50</v>
@@ -784,7 +787,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2">
         <v>5.0000000000000004E-6</v>
@@ -801,30 +804,30 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="1">
-        <v>2000</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2000</v>
-      </c>
-      <c r="D20" s="1">
-        <v>298</v>
-      </c>
-      <c r="E20" s="1">
-        <v>298</v>
+        <v>30</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1">
-        <v>298</v>
+        <v>2000</v>
       </c>
       <c r="C21" s="1">
-        <v>298</v>
+        <v>2000</v>
       </c>
       <c r="D21" s="1">
         <v>298</v>
@@ -835,35 +838,52 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1">
-        <v>4</v>
+        <v>298</v>
       </c>
       <c r="C22" s="1">
-        <v>4</v>
+        <v>298</v>
       </c>
       <c r="D22" s="1">
-        <v>4</v>
+        <v>298</v>
       </c>
       <c r="E22" s="1">
-        <v>4</v>
+        <v>298</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1">
         <v>0.1</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C24" s="1">
         <v>0.1</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D24" s="1">
         <v>0.1</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E24" s="1">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>